<commit_message>
adding featherlook1.0 shoudl probably be 1.1 because it works as an executable and does not do the notepade copy for searchword(which may be the same as the last one on master?), adding log, and .gitignore (which has more things added to it)
</commit_message>
<xml_diff>
--- a/featherlook_log.xlsx
+++ b/featherlook_log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Featherlook progress log</t>
   </si>
@@ -62,7 +62,10 @@
     <t>parsed into sentences</t>
   </si>
   <si>
-    <t>My next steps: 1) remove file path  only need file name, 2) see if I can do without the little tk window; 3) output window scroll bar; 4) output window copy-able; 5)put into a stand alone .exe</t>
+    <t>My next steps: 1) remove file path  only need file name, 2) see if I can do without the little tk window; 3) output window scroll bar; 4) output window copy-able; 5)put into a stand alone .exe; 6) make a function for parsinng paragraph to sentence</t>
+  </si>
+  <si>
+    <t>completed #4 and #6 in previous next steps. made parsing paragraph to sentence a function and hide little window that is used to bring up .askdialog prompt.</t>
   </si>
 </sst>
 </file>
@@ -381,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,6 +452,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>43839</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Major chnage is featherlook written to run from an executable. Minor is there is a popup that tells path which i will remove, but iwant to keep in this version incase i run into more path and executable issues
</commit_message>
<xml_diff>
--- a/featherlook_log.xlsx
+++ b/featherlook_log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Featherlook progress log</t>
   </si>
@@ -66,6 +66,13 @@
   </si>
   <si>
     <t>completed #4 and #6 in previous next steps. made parsing paragraph to sentence a function and hide little window that is used to bring up .askdialog prompt.</t>
+  </si>
+  <si>
+    <t>Major development: script is set up to run from executable on Windows. 
+Minor:This version includes a popup that shows the absolute path for the temporary file I make to store the search word so I don't have to use .get() all over the place.</t>
+  </si>
+  <si>
+    <t>1)remove popup for path; 2)add scroll; 3) limit size of lists so that users don't select directory with large search and run takes forever - this is just a toy; 4)describe function of app so its obvious for user what this is. Maybe add popup or labels to guide</t>
   </si>
 </sst>
 </file>
@@ -101,9 +108,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,6 +471,20 @@
         <v>13</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>43842</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Major development: recreated file search and parser with limits. I kind of know what's going on. Minor development: its not in a separate function
</commit_message>
<xml_diff>
--- a/featherlook_log.xlsx
+++ b/featherlook_log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Featherlook progress log</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>1)remove popup for path; 2)add scroll; 3) limit size of lists so that users don't select directory with large search and run takes forever - this is just a toy; 4)describe function of app so its obvious for user what this is. Maybe add popup or labels to guide</t>
+  </si>
+  <si>
+    <t>Major development: recreated file search and parser with limits. I kind of know what's going on. Minor development: its not in a separate function</t>
   </si>
 </sst>
 </file>
@@ -392,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,6 +488,17 @@
         <v>15</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>43843</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
i think i've made a mess
</commit_message>
<xml_diff>
--- a/featherlook_log.xlsx
+++ b/featherlook_log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Featherlook progress log</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>1)remove popup for path; 2)add scroll; 3) limit size of lists so that users don't select directory with large search and run takes forever - this is just a toy; 4)describe function of app so its obvious for user what this is. Maybe add popup or labels to guide</t>
-  </si>
-  <si>
-    <t>Major development: recreated file search and parser with limits. I kind of know what's going on. Minor development: its not in a separate function</t>
   </si>
 </sst>
 </file>
@@ -395,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,17 +485,6 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
-        <v>43843</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>